<commit_message>
Update Skype Lab B Final Solution
</commit_message>
<xml_diff>
--- a/O3659/O3659-2 OfficeAddinWebSDK/Final Solution/OfficeAddIn/TestPayroll.xlsx
+++ b/O3659/O3659-2 OfficeAddinWebSDK/Final Solution/OfficeAddIn/TestPayroll.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Skype Build Demo\Build 2016\POC\OfficeAddIn\OfficeAddIn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troberts\Downloads\Lab B\Lab B\Lab B - Final\OfficeAddIn\OfficeAddIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,16 +29,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>marysmith@claritydemo.ccsctp.net</t>
+    <t>User1@contoso.onmicrosoft.com</t>
   </si>
   <si>
-    <t>johnarmstrong@claritydemo.ccsctp.net</t>
+    <t>User2@contoso.onmicrosoft.com</t>
   </si>
   <si>
-    <t>davidberg@claritydemo.ccsctp.net</t>
+    <t>User3@contoso.onmicrosoft.com</t>
   </si>
   <si>
-    <t>billanderson@claritydemo.ccsctp.net</t>
+    <t>User4@contoso.onmicrosoft.com</t>
   </si>
 </sst>
 </file>
@@ -85,7 +85,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -388,7 +390,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -418,10 +420,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A1" r:id="rId1" display="mailto:User1@contoso.onmicrosoft.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="mailto:User2@contoso.onmicrosoft.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="mailto:User3@contoso.onmicrosoft.com"/>
+    <hyperlink ref="A4" r:id="rId4" display="mailto:User4@contoso.onmicrosoft.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>